<commit_message>
trả thêm store status
</commit_message>
<xml_diff>
--- a/DMS/Templates/Report_Statistic_Problem.xlsx
+++ b/DMS/Templates/Report_Statistic_Problem.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rang Dong\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EE1859-930C-45C7-A166-35EE207AD9FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7215E9-8ED2-4F14-ACD2-B79ECFD40518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>STT</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>{{ReportStatisticProblems.Stores.Contents.Total}}</t>
+  </si>
+  <si>
+    <t>Trạng thái đại lý</t>
+  </si>
+  <si>
+    <t>{{ReportStatisticProblems.Stores.StoreStatus.Name}}</t>
   </si>
 </sst>
 </file>
@@ -250,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -270,23 +276,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -304,11 +304,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,230 +612,250 @@
     <col min="4" max="4" width="5.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="9" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="6"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
       <c r="F2" s="5"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
-    <row r="4" spans="1:25" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:27" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="14"/>
       <c r="K5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="4"/>
+      <c r="O5" s="4"/>
     </row>
-    <row r="7" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="19" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="19" t="s">
+      <c r="F7" s="18"/>
+      <c r="G7" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="18"/>
+      <c r="I7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="19" t="s">
+      <c r="J7" s="18"/>
+      <c r="K7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="18"/>
+      <c r="M7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="18"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="16"/>
     </row>
-    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="12" t="s">
+      <c r="D9" s="23"/>
+      <c r="E9" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12" t="s">
+      <c r="F9" s="23"/>
+      <c r="G9" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="23"/>
+      <c r="I9" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="12" t="s">
+      <c r="J9" s="23"/>
+      <c r="K9" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="8" t="s">
+      <c r="L9" s="23"/>
+      <c r="M9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="21" t="s">
+      <c r="N9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="21" t="s">
+      <c r="O9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="P9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="O9" s="21" t="s">
+      <c r="Q9" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:27" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="22" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="O10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="22" t="s">
+      <c r="P10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="22" t="s">
+      <c r="Q10" s="12" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A8:Y8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A4:O4"/>
+  <mergeCells count="17">
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A4:Q4"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:AA8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>